<commit_message>
added few more test cases with fail
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04699E3E-7A57-A046-A4BB-0B8548C3359B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE4F9F8-7F7D-4840-BCB5-6FE0733EC9AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,25 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>zipCode</t>
-  </si>
-  <si>
-    <t>Chand</t>
-  </si>
-  <si>
-    <t>Birendra</t>
-  </si>
-  <si>
-    <t>Bivek</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>emailAddress</t>
   </si>
@@ -59,7 +42,19 @@
     <t>abctest@test.com</t>
   </si>
   <si>
-    <t>helo@test.com</t>
+    <t>bbb@bbb.com</t>
+  </si>
+  <si>
+    <t>bbbbb</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>passWord</t>
+  </si>
+  <si>
+    <t>baa@bbb.com</t>
   </si>
 </sst>
 </file>
@@ -422,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,52 +428,62 @@
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>11111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>22222</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F57CC7E4-3D4E-A047-9CDC-D247ED949AC2}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{AEB4355D-A7F1-8343-98A9-459CFF0C81C2}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{AD203446-9358-C44E-A250-75BF80F4BA1A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41A1671-81ED-9449-8E25-F8FC946C243B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3CF84504-2C24-0642-B8D9-C826669A5B07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added run mode to skip or run a test case
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE4F9F8-7F7D-4840-BCB5-6FE0733EC9AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D769598-1C64-F341-8AE0-3721F6171E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="28040" windowHeight="16240" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Parameter" sheetId="3" r:id="rId3"/>
+    <sheet name="test_suite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>emailAddress</t>
   </si>
@@ -55,13 +57,49 @@
   </si>
   <si>
     <t>baa@bbb.com</t>
+  </si>
+  <si>
+    <t>ccc@ccc.com</t>
+  </si>
+  <si>
+    <t>ccccc</t>
+  </si>
+  <si>
+    <t>eee@eee.com</t>
+  </si>
+  <si>
+    <t>eeeee</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Ordering</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>VerifyLoginPage</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,6 +114,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,9 +143,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -419,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -457,7 +502,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,4 +532,119 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C7F4AD-25ED-8742-9191-B6AEC26E727B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9F351E4B-3150-5F44-AE6E-6B6B80D65048}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{CE426EE1-501A-BD40-9C41-38A9FB0E5ECD}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{38F46F81-1A78-DC47-B2FE-5D9E0EA2552F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added method to generate random data, data provider to read the random data
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D769598-1C64-F341-8AE0-3721F6171E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6D646B-0564-2440-AE06-55E1CB801407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="28040" windowHeight="16240" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Parameter" sheetId="3" r:id="rId3"/>
-    <sheet name="test_suite" sheetId="4" r:id="rId4"/>
+    <sheet name="random" sheetId="7" r:id="rId4"/>
+    <sheet name="test_suite" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>emailAddress</t>
   </si>
   <si>
-    <t>abctest@test.com</t>
-  </si>
-  <si>
     <t>bbb@bbb.com</t>
   </si>
   <si>
@@ -56,9 +54,6 @@
     <t>passWord</t>
   </si>
   <si>
-    <t>baa@bbb.com</t>
-  </si>
-  <si>
     <t>ccc@ccc.com</t>
   </si>
   <si>
@@ -89,16 +84,41 @@
     <t>VerifyLoginPage</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>fsd@kk.com</t>
+  </si>
+  <si>
+    <t>kdkffsfk</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>lld</t>
+  </si>
+  <si>
+    <t>bivek</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>jfqn@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -464,13 +484,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -480,19 +499,15 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F57CC7E4-3D4E-A047-9CDC-D247ED949AC2}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{AD203446-9358-C44E-A250-75BF80F4BA1A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -507,23 +522,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -536,48 +551,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C7F4AD-25ED-8742-9191-B6AEC26E727B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -585,44 +606,73 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{9F351E4B-3150-5F44-AE6E-6B6B80D65048}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{CE426EE1-501A-BD40-9C41-38A9FB0E5ECD}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{38F46F81-1A78-DC47-B2FE-5D9E0EA2552F}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{62287CC3-9AAF-CE4E-A0E4-B75C7427D17A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6040F15B-764C-AA4D-9CF7-90EA30C035A4}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3359375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -630,17 +680,25 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "added method to generate random data, data provider to read the random data"
This reverts commit 41535184472924d84b1130ff747a213b91bc6d24.
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -3,25 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6D646B-0564-2440-AE06-55E1CB801407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D769598-1C64-F341-8AE0-3721F6171E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="28040" windowHeight="16240" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Parameter" sheetId="3" r:id="rId3"/>
-    <sheet name="random" sheetId="7" r:id="rId4"/>
-    <sheet name="test_suite" sheetId="4" r:id="rId5"/>
+    <sheet name="test_suite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,11 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>emailAddress</t>
   </si>
   <si>
+    <t>abctest@test.com</t>
+  </si>
+  <si>
     <t>bbb@bbb.com</t>
   </si>
   <si>
@@ -54,6 +56,9 @@
     <t>passWord</t>
   </si>
   <si>
+    <t>baa@bbb.com</t>
+  </si>
+  <si>
     <t>ccc@ccc.com</t>
   </si>
   <si>
@@ -84,41 +89,16 @@
     <t>VerifyLoginPage</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Registration</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>fsd@kk.com</t>
-  </si>
-  <si>
-    <t>kdkffsfk</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>lld</t>
-  </si>
-  <si>
-    <t>bivek</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>jfqn@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -484,12 +464,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -499,15 +480,19 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F57CC7E4-3D4E-A047-9CDC-D247ED949AC2}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{AD203446-9358-C44E-A250-75BF80F4BA1A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -522,23 +507,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -551,54 +536,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C7F4AD-25ED-8742-9191-B6AEC26E727B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -606,73 +585,44 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{9F351E4B-3150-5F44-AE6E-6B6B80D65048}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{CE426EE1-501A-BD40-9C41-38A9FB0E5ECD}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{38F46F81-1A78-DC47-B2FE-5D9E0EA2552F}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{62287CC3-9AAF-CE4E-A0E4-B75C7427D17A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6040F15B-764C-AA4D-9CF7-90EA30C035A4}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3359375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -680,25 +630,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "added method to generate random data, data provider to read the random data""
This reverts commit 01b8dc50a451bdd3369acbd39cc192d84a72ca76.
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D769598-1C64-F341-8AE0-3721F6171E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6D646B-0564-2440-AE06-55E1CB801407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="28040" windowHeight="16240" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Parameter" sheetId="3" r:id="rId3"/>
-    <sheet name="test_suite" sheetId="4" r:id="rId4"/>
+    <sheet name="random" sheetId="7" r:id="rId4"/>
+    <sheet name="test_suite" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>emailAddress</t>
   </si>
   <si>
-    <t>abctest@test.com</t>
-  </si>
-  <si>
     <t>bbb@bbb.com</t>
   </si>
   <si>
@@ -56,9 +54,6 @@
     <t>passWord</t>
   </si>
   <si>
-    <t>baa@bbb.com</t>
-  </si>
-  <si>
     <t>ccc@ccc.com</t>
   </si>
   <si>
@@ -89,16 +84,41 @@
     <t>VerifyLoginPage</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>fsd@kk.com</t>
+  </si>
+  <si>
+    <t>kdkffsfk</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>lld</t>
+  </si>
+  <si>
+    <t>bivek</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>jfqn@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -464,13 +484,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -480,19 +499,15 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F57CC7E4-3D4E-A047-9CDC-D247ED949AC2}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{AD203446-9358-C44E-A250-75BF80F4BA1A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -507,23 +522,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -536,48 +551,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C7F4AD-25ED-8742-9191-B6AEC26E727B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -585,44 +606,73 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{9F351E4B-3150-5F44-AE6E-6B6B80D65048}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{CE426EE1-501A-BD40-9C41-38A9FB0E5ECD}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{38F46F81-1A78-DC47-B2FE-5D9E0EA2552F}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{62287CC3-9AAF-CE4E-A0E4-B75C7427D17A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6040F15B-764C-AA4D-9CF7-90EA30C035A4}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3359375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -630,17 +680,25 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added function to generate random test data
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>emailAddress</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>jfqn@test.com</t>
+  </si>
+  <si>
+    <t>jzdh@test.com</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.3359375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.92578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -632,7 +635,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test case to use data provider
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6D646B-0564-2440-AE06-55E1CB801407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69251A6F-F71E-BB43-9406-FBAF93C120A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>emailAddress</t>
   </si>
@@ -90,31 +90,22 @@
     <t>Registration</t>
   </si>
   <si>
+    <t>fsd@kk.com</t>
+  </si>
+  <si>
+    <t>kdkffsfk</t>
+  </si>
+  <si>
+    <t>foxh@test.com</t>
+  </si>
+  <si>
+    <t>cfwu@test.com</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>fsd@kk.com</t>
-  </si>
-  <si>
-    <t>kdkffsfk</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>lld</t>
-  </si>
-  <si>
-    <t>bivek</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>jfqn@test.com</t>
-  </si>
-  <si>
-    <t>jzdh@test.com</t>
+    <t>oshz@test.com</t>
   </si>
 </sst>
 </file>
@@ -485,13 +476,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.6328125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -502,12 +495,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +508,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,10 +586,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -619,23 +607,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6040F15B-764C-AA4D-9CF7-90EA30C035A4}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.92578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -647,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +666,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -686,7 +674,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -694,7 +682,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -702,7 +690,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the email report from IP to localhost
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69251A6F-F71E-BB43-9406-FBAF93C120A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D264CE-1014-6044-B02B-FE8C9618F3A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="3" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>emailAddress</t>
   </si>
@@ -99,13 +99,64 @@
     <t>foxh@test.com</t>
   </si>
   <si>
-    <t>cfwu@test.com</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>oshz@test.com</t>
+    <t>bcwe@test.com</t>
+  </si>
+  <si>
+    <t>nmko@test.com</t>
+  </si>
+  <si>
+    <t>lekn@test.com</t>
+  </si>
+  <si>
+    <t>ejyg@test.com</t>
+  </si>
+  <si>
+    <t>swjf@test.com</t>
+  </si>
+  <si>
+    <t>jseh@test.com</t>
+  </si>
+  <si>
+    <t>bryl@test.com</t>
+  </si>
+  <si>
+    <t>ngqj@test.com</t>
+  </si>
+  <si>
+    <t>wsvf@test.com</t>
+  </si>
+  <si>
+    <t>rzfs@test.com</t>
+  </si>
+  <si>
+    <t>szhn@test.com</t>
+  </si>
+  <si>
+    <t>bnih@test.com</t>
+  </si>
+  <si>
+    <t>ofad@test.com</t>
+  </si>
+  <si>
+    <t>xjrj@test.com</t>
+  </si>
+  <si>
+    <t>pswq@test.com</t>
+  </si>
+  <si>
+    <t>zumx@test.com</t>
+  </si>
+  <si>
+    <t>nclj@test.com</t>
+  </si>
+  <si>
+    <t>dnlw@test.com</t>
+  </si>
+  <si>
+    <t>olkn@test.com</t>
   </si>
 </sst>
 </file>
@@ -484,7 +535,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.6328125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.69921875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -495,7 +546,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6040F15B-764C-AA4D-9CF7-90EA30C035A4}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -635,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -666,7 +717,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -674,7 +725,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -682,7 +733,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
turned on some tests on suite
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>emailAddress</t>
   </si>
@@ -103,12 +103,19 @@
   </si>
   <si>
     <t>whha@test.com</t>
+  </si>
+  <si>
+    <t>eibq@test.com</t>
+  </si>
+  <si>
+    <t>zqio@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -472,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -480,8 +487,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.34765625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -491,7 +498,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -509,7 +516,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -544,8 +551,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -609,7 +616,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -637,8 +644,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed values on test mode
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02C1E7B-CF92-4C45-95FA-F411022DAB3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBAA569-9A6C-EB47-BC38-EEA8F610E66A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>emailAddress</t>
   </si>
@@ -99,16 +99,16 @@
     <t>foxh@test.com</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>whha@test.com</t>
-  </si>
-  <si>
-    <t>eibq@test.com</t>
-  </si>
-  <si>
-    <t>zqio@test.com</t>
+    <t>fqro@test.com</t>
+  </si>
+  <si>
+    <t>thht@test.com</t>
+  </si>
+  <si>
+    <t>uiuu@test.com</t>
+  </si>
+  <si>
+    <t>dowr@test.com</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.34765625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -639,7 +639,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -685,7 +685,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed values in excel
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBAA569-9A6C-EB47-BC38-EEA8F610E66A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C35560-D92C-2D4A-9CA8-0767BC4B7991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>emailAddress</t>
   </si>
@@ -99,23 +99,16 @@
     <t>foxh@test.com</t>
   </si>
   <si>
-    <t>fqro@test.com</t>
-  </si>
-  <si>
-    <t>thht@test.com</t>
-  </si>
-  <si>
-    <t>uiuu@test.com</t>
-  </si>
-  <si>
     <t>dowr@test.com</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -479,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -487,8 +480,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -498,7 +491,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -516,7 +509,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -551,8 +544,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -616,7 +609,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -639,13 +632,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -669,7 +662,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -677,7 +670,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -685,7 +678,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -693,7 +686,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Docker run, changed xml file
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>emailAddress</t>
   </si>
@@ -100,12 +100,25 @@
   </si>
   <si>
     <t>ypqh@test.com</t>
+  </si>
+  <si>
+    <t>tdia@test.com</t>
+  </si>
+  <si>
+    <t>kxbh@test.com</t>
+  </si>
+  <si>
+    <t>ohge@test.com</t>
+  </si>
+  <si>
+    <t>wjhk@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -469,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -477,8 +490,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.87890625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -488,7 +501,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -506,7 +519,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -541,8 +554,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -606,7 +619,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -634,8 +647,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
removed random tab from excel
</commit_message>
<xml_diff>
--- a/SampleDataTest/src/test/resources/excel/testdata.xlsx
+++ b/SampleDataTest/src/test/resources/excel/testdata.xlsx
@@ -3,25 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birendra/git/datadriven/SampleDataTest/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A25FEFF-966A-2347-A66D-EEA660C32EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CC3CB3-D634-B646-8786-09866FFDEE6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="2" xr2:uid="{D4C29085-3C51-A843-BD80-F2FB7D7A8223}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Parameter" sheetId="3" r:id="rId3"/>
-    <sheet name="random" sheetId="7" r:id="rId4"/>
-    <sheet name="test_suite" sheetId="4" r:id="rId5"/>
+    <sheet name="test_suite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>emailAddress</t>
   </si>
@@ -96,29 +95,13 @@
     <t>kdkffsfk</t>
   </si>
   <si>
-    <t>foxh@test.com</t>
-  </si>
-  <si>
-    <t>ypqh@test.com</t>
-  </si>
-  <si>
-    <t>tdia@test.com</t>
-  </si>
-  <si>
-    <t>kxbh@test.com</t>
-  </si>
-  <si>
-    <t>ohge@test.com</t>
-  </si>
-  <si>
-    <t>wjhk@test.com</t>
+    <t>vjgp@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -482,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FC4D48-DC78-584B-A653-3D520D4D2EC2}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -490,8 +473,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.87890625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -501,7 +484,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -519,7 +502,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -550,12 +533,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C7F4AD-25ED-8742-9191-B6AEC26E727B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -610,45 +593,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6040F15B-764C-AA4D-9CF7-90EA30C035A4}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.83203125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3673646B-5788-E24B-8703-0F69FA5EFCC7}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>